<commit_message>
with pdf view and resend email
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashbeemorgado/devs/payslip/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47702212-14D3-D24B-8511-B018EC0DB73E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871C22EC-84CA-2D48-97BD-2E4F05844517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Wuclq9pgLSwiCN1CxHFBNWf9x6XLXGbE6cpp/enLMmLVbkGbIcMtVXlukoDUpBB7FAg5JO25g2YiiEzjFoLAdA==" workbookSaltValue="tK63htd/GaSpK8v4Ie3M4Q==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20920" xr2:uid="{8ED9818E-59F9-6949-8D1A-5036E9068AA9}"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>No.</t>
   </si>
@@ -172,61 +172,61 @@
     <t>E-mail Address</t>
   </si>
   <si>
+    <t>Days Worked</t>
+  </si>
+  <si>
+    <t>Days Absent</t>
+  </si>
+  <si>
+    <t>Absent Amount</t>
+  </si>
+  <si>
+    <t>Tardiness Amount</t>
+  </si>
+  <si>
+    <t>Overtime Pay</t>
+  </si>
+  <si>
+    <t>Others/Remarks Addition Amount</t>
+  </si>
+  <si>
+    <t>Total Deductions</t>
+  </si>
+  <si>
+    <t>Holiday Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MORGADO, JOHN ASHBEE A. </t>
+  </si>
+  <si>
+    <t>MAY 16-31</t>
+  </si>
+  <si>
+    <t>SSS Contribution</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>PHIC Contribution</t>
+  </si>
+  <si>
+    <t>HDMF Contribution</t>
+  </si>
+  <si>
+    <t>ashbeemorgado11@gmail.com</t>
+  </si>
+  <si>
+    <t>GROSS COMPENSATION</t>
+  </si>
+  <si>
+    <t>TAXABLE COMPENSATION</t>
+  </si>
+  <si>
     <t>Start Date</t>
   </si>
   <si>
-    <t>Cuf-Off Date</t>
-  </si>
-  <si>
-    <t>Days Worked</t>
-  </si>
-  <si>
-    <t>Days Absent</t>
-  </si>
-  <si>
-    <t>Absent Amount</t>
-  </si>
-  <si>
-    <t>Tardiness Amount</t>
-  </si>
-  <si>
-    <t>Overtime Pay</t>
-  </si>
-  <si>
-    <t>Others/Remarks Addition Amount</t>
-  </si>
-  <si>
-    <t>Total Deductions</t>
-  </si>
-  <si>
-    <t>Holiday Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MORGADO, JOHN ASHBEE A. </t>
-  </si>
-  <si>
-    <t>MAY 16-31</t>
-  </si>
-  <si>
-    <t>SSS Contribution</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>PHIC Contribution</t>
-  </si>
-  <si>
-    <t>HDMF Contribution</t>
-  </si>
-  <si>
-    <t>ashbeemorgado11@gmail.com</t>
-  </si>
-  <si>
-    <t>GROSS COMPENSATION</t>
-  </si>
-  <si>
-    <t>TAXABLE COMPENSATION</t>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
@@ -237,7 +237,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mmm\ dd\,\ yyyy\ ddd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -292,14 +292,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -397,24 +389,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -425,12 +407,22 @@
     <xf numFmtId="43" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -452,10 +444,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -768,439 +760,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC76FFC-1A64-1341-A4F3-70BB52FA1105}">
-  <dimension ref="A1:AO7"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:H22"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="AL9" sqref="AL9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="12"/>
-    <col min="5" max="5" width="13.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.83203125" style="12"/>
-    <col min="12" max="12" width="13.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="12"/>
-    <col min="14" max="14" width="17.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="13"/>
-    <col min="16" max="16" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="12"/>
-    <col min="18" max="18" width="14.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5" style="13" customWidth="1"/>
-    <col min="28" max="28" width="17.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="11" style="13" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.83203125" style="12"/>
-    <col min="38" max="38" width="0" style="12" hidden="1" customWidth="1"/>
-    <col min="39" max="40" width="16.5" style="2" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="16.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="26.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="14" width="17.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="4"/>
+    <col min="16" max="16" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="3"/>
+    <col min="18" max="18" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5" style="4" customWidth="1"/>
+    <col min="28" max="28" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.83203125" style="3" customWidth="1"/>
+    <col min="39" max="39" width="16.5" style="12" customWidth="1"/>
+    <col min="40" max="41" width="16.5" style="3" hidden="1" customWidth="1"/>
+    <col min="42" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="24">
+      <c r="D1" s="17">
         <v>43962</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="7"/>
-      <c r="AN1" s="7"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B2" s="4"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="17">
         <v>43976</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="28" t="s">
+      <c r="K3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="28" t="s">
+      <c r="L3" s="22"/>
+      <c r="M3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="29"/>
-      <c r="O3" s="15" t="s">
+      <c r="N3" s="22"/>
+      <c r="O3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="Q3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20" t="s">
+      <c r="R3" s="10"/>
+      <c r="S3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="T3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="26"/>
-      <c r="W3" s="27"/>
-      <c r="X3" s="15" t="s">
+      <c r="V3" s="19"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Y3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Z3" s="25" t="s">
+      <c r="Z3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="26"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="27"/>
-      <c r="AK3" s="15" t="s">
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="19"/>
+      <c r="AJ3" s="20"/>
+      <c r="AK3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="29"/>
-      <c r="AN3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO3" s="11" t="s">
-        <v>47</v>
-      </c>
+      <c r="AL3" s="21"/>
+      <c r="AM3" s="22"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="16" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="16" t="s">
+      <c r="M4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="O4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="17" t="s">
+      <c r="T4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="W4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="17" t="s">
+      <c r="X4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="T4" s="17" t="s">
+      <c r="AO4" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="U4" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="X4" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z4" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA4" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD4" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF4" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG4" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH4" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK4" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="AL4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN4" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO4" s="18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B5" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="13">
+      <c r="F5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="4">
         <v>24100</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="4">
         <v>1095.4545000000001</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="3">
         <v>11</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="3">
         <v>12050</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="4">
         <v>12050</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="4">
         <v>12050</v>
       </c>
-      <c r="U5" s="13">
+      <c r="U5" s="4">
         <v>2000</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="4">
         <v>5000</v>
       </c>
-      <c r="Y5" s="13">
+      <c r="Y5" s="4">
         <v>12050</v>
       </c>
-      <c r="Z5" s="13">
+      <c r="Z5" s="4">
         <v>200.45</v>
       </c>
-      <c r="AA5" s="13">
+      <c r="AA5" s="4">
         <v>800</v>
       </c>
-      <c r="AC5" s="13">
+      <c r="AC5" s="4">
         <v>100</v>
       </c>
-      <c r="AD5" s="13">
+      <c r="AD5" s="4">
         <v>315</v>
       </c>
-      <c r="AF5" s="13">
+      <c r="AF5" s="4">
         <v>807.54</v>
       </c>
-      <c r="AH5" s="13">
+      <c r="AH5" s="4">
         <v>500</v>
       </c>
-      <c r="AJ5" s="12">
+      <c r="AJ5" s="3">
         <v>3084.49</v>
       </c>
-      <c r="AK5" s="12">
+      <c r="AK5" s="3">
         <v>8965.51</v>
       </c>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3">
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="23">
         <f>D1</f>
         <v>43962</v>
       </c>
-      <c r="AO5" s="3">
+      <c r="AO5" s="23">
         <f>D2</f>
         <v>43976</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="B7" s="22"/>
-      <c r="J7" s="23"/>
-      <c r="AK7" s="23"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mCWGnTF4cUj5n2NEwM2LmbEdGL9efI/9SOlRIgMkfswS9u53OL+2OioLBUs1r3BUy6GLzpkI7+08xL3KpkH4mw==" saltValue="EN7PrrGpiJ6mcFTQ0oi5Qg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mwdXdWAFsUkBSiTaeuo+57EMreqjW2rPwoO3uEKL4d1VZiaVDYclHhkRt2hQZA7TGa1y3WJ6hqeC5Z+UUIrKWw==" saltValue="CShlNbKXNf96QMhROYd4jg==" spinCount="100000" sheet="1" objects="1" scenarios="1" deleteRows="0"/>
   <mergeCells count="7">
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D2:G2"/>

</xml_diff>